<commit_message>
worked out problems related to uploading large files
</commit_message>
<xml_diff>
--- a/src/test/resources/SpreadsheetForReadingTest.xlsx
+++ b/src/test/resources/SpreadsheetForReadingTest.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet Containing Data" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -79,6 +79,104 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -88,83 +186,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -172,29 +195,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -209,12 +209,165 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
     <fill>
@@ -224,160 +377,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -387,6 +387,36 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -417,17 +447,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -449,45 +488,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -499,47 +499,47 @@
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -898,105 +898,126 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1">
+        <v>1.5</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>42005</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>42006</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="C4" s="1">
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
         <v>42007</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>3.3450000000000002</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>9</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>10</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D7" s="1">
         <v>42009</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F7" t="s">
         <v>12</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J7" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>